<commit_message>
Finishing touches and running scenarios
</commit_message>
<xml_diff>
--- a/Parameters/conversion_parameters.xlsx
+++ b/Parameters/conversion_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mans3904/Documents/GitHub/GEOH2-private/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ls2823_ic_ac_uk/Documents/0_Thesis/0relevant_repositories/GeoH2 Case Study Laos/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D70AFA-7E5E-B047-8AF2-268A0DA8727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{F3D70AFA-7E5E-B047-8AF2-268A0DA8727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{684514E5-0D9D-4BE7-A558-9BB722749078}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="14820" windowHeight="14480" activeTab="3" xr2:uid="{18B0DDC9-B74C-4E09-B886-3EB1C823232B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{18B0DDC9-B74C-4E09-B886-3EB1C823232B}"/>
   </bookViews>
   <sheets>
     <sheet name="500 bar" sheetId="1" r:id="rId1"/>
@@ -70,43 +70,43 @@
     <t>Electricity demand (kWh per kg H2)</t>
   </si>
   <si>
-    <t>Capex quadratic coefficient (euros (kg H2)-2)</t>
-  </si>
-  <si>
-    <t>Capex linear coefficient (euros per kg H2)</t>
-  </si>
-  <si>
-    <t>Capex constant (euros)</t>
-  </si>
-  <si>
     <t>Opex (% of capex)</t>
   </si>
   <si>
     <t>Plant lifetime (a)</t>
   </si>
   <si>
-    <t>Compressor capex coefficient (euros per kilograms H2 per day)</t>
-  </si>
-  <si>
     <t>Heat demand (kWh per kg H2)</t>
   </si>
   <si>
-    <t>Capex coefficient (euros per kilograms H2 per year)</t>
-  </si>
-  <si>
     <t>Hydrogenation lifetime (a)</t>
   </si>
   <si>
-    <t>Carrier costs (euros per kg carrier)</t>
-  </si>
-  <si>
-    <t>Capex coefficient (euros per annual g H2)</t>
-  </si>
-  <si>
-    <t>Capex coefficient (euros per hourly g H2)</t>
-  </si>
-  <si>
     <t>Carrier ratio (kg carrier: kg hydrogen)</t>
+  </si>
+  <si>
+    <t>Compressor capex coefficient (USD per kilograms H2 per day)</t>
+  </si>
+  <si>
+    <t>Capex quadratic coefficient (USD (kg H2)-2)</t>
+  </si>
+  <si>
+    <t>Capex linear coefficient (USD per kg H2)</t>
+  </si>
+  <si>
+    <t>Capex constant (USD)</t>
+  </si>
+  <si>
+    <t>Capex coefficient (USD per kilograms H2 per year)</t>
+  </si>
+  <si>
+    <t>Carrier costs (USD per kg carrier)</t>
+  </si>
+  <si>
+    <t>Capex coefficient (USD per annual g H2)</t>
+  </si>
+  <si>
+    <t>Capex coefficient (USD per hourly g H2)</t>
   </si>
 </sst>
 </file>
@@ -162,9 +162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -202,7 +202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -308,7 +308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -450,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,20 +461,20 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -483,7 +483,7 @@
         <v>3.9444447600000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -491,7 +491,7 @@
         <v>298.14999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -499,7 +499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -507,7 +507,7 @@
         <v>1.4019999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -515,7 +515,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -523,15 +523,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>40035</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -549,21 +549,22 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -571,42 +572,41 @@
         <v>9.93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>1781.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1877.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <f>3*(100000000)</f>
-        <v>300000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>317400000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -621,19 +621,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15D9C4-0313-4761-ABC1-34D86A7C1894}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -641,49 +643,49 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.1160000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>16.100000000000001</v>
@@ -696,120 +698,57 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE59E596-5506-44A6-B32A-5A1FC3D73A2D}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>2.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E224CE-91BF-435F-A756-EB96A1C22628}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <v>2.8090000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>0.75717000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>12</v>
-      </c>
-      <c r="B5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
       </c>
       <c r="B6">
         <v>25</v>
@@ -820,25 +759,88 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E224CE-91BF-435F-A756-EB96A1C22628}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>2.8090000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.797906</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBAAF98-B70E-424E-84FC-CE6118F32624}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -846,34 +848,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <f>18.171 * 0.95 * 1000000</f>
-        <v>17262449.999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18191170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>25</v>

</xml_diff>